<commit_message>
Metodo Open 29May2019 21H
</commit_message>
<xml_diff>
--- a/Documentacion.xlsx
+++ b/Documentacion.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7106CA0-ED44-4B56-8B3B-3950830DD69C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comandos" sheetId="1" r:id="rId1"/>
     <sheet name="EtapaAnalisisDatos" sheetId="2" r:id="rId2"/>
     <sheet name="ModelosPredictivos" sheetId="3" r:id="rId3"/>
     <sheet name="DataScientist" sheetId="4" r:id="rId4"/>
+    <sheet name="DataClean" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Actualizar Pip</t>
   </si>
@@ -117,18 +119,41 @@
   <si>
     <t xml:space="preserve"> Los modelos predictivos  sigue un principio básico de la estadística que es la regla de Paret,las cosas importantes de la vida se dividen siempre en la regla del 80 20.</t>
   </si>
+  <si>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Es un fichero o estructura de datos que contine informacion organizada generalmente con filas y columnas, ejm una tabla SQL o una tabla de Excel</t>
+  </si>
+  <si>
+    <t>Siempre contienen un delimitar que separa los datos, generalmente es la ","</t>
+  </si>
+  <si>
+    <t>Funcion Open</t>
+  </si>
+  <si>
+    <t>A diferencia de read_csv que carga todos los datos de una sola vez ocupando gran parte de la memoria , este lee el archivo line apor linea
+mediante un ciclo for y elimina de la memoria la esra informacion una vez ha sido procesada</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF007791"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,12 +182,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,11 +835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,6 +917,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -898,7 +932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
@@ -911,7 +945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:I51"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -985,10 +1019,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1003,4 +1037,33 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A580862-A30C-4D05-8A3E-54C77674BE80}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>